<commit_message>
Remove unnecessary columns from imaging templates
</commit_message>
<xml_diff>
--- a/templates/2EXT05_Imaging.xlsx
+++ b/templates/2EXT05_Imaging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\omaus\SWATE_templates\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cremp\Documents\GitHub\SWATE_templates\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2239E11B-FDD2-4220-8F7C-AC8E555EFBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B832287-E8EC-4BC9-8247-8EC1C23F04C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2EXT05_Imaging" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -44,12 +42,21 @@
   <commentList>
     <comment ref="A1" authorId="0" shapeId="0" xr:uid="{9067AD98-F807-46F1-B65C-78D939534A6A}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     The unique identifier of this template. It will be auto generated.
 Reply:
     id=8fbc694a-5adf-4f97-8cd8-3bcedc37c98d</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -57,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="366">
   <si>
     <t>Source Name</t>
   </si>
@@ -74,33 +81,12 @@
     <t>Term Accession Number (NFDI4PSO:1000143)</t>
   </si>
   <si>
-    <t>Parameter [prepared organism part]</t>
-  </si>
-  <si>
     <t>Term Source REF (NFDI4PSO:1000145)</t>
   </si>
   <si>
     <t>Term Accession Number (NFDI4PSO:1000145)</t>
   </si>
   <si>
-    <t>Parameter [Microscopy study type]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:1000139)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000139)</t>
-  </si>
-  <si>
-    <t>Parameter [experiment name]</t>
-  </si>
-  <si>
-    <t>Term Source REF (MS:1002120)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (MS:1002120)</t>
-  </si>
-  <si>
     <t>Parameter [generic experimental condition]</t>
   </si>
   <si>
@@ -209,15 +195,6 @@
     <t>Term Accession Number (NFDI4PSO:1000119)</t>
   </si>
   <si>
-    <t>Parameter [Screen Technology Type]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NFDI4PSO:1000114)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NFDI4PSO:1000114)</t>
-  </si>
-  <si>
     <t>Parameter [high content screening stage]</t>
   </si>
   <si>
@@ -629,21 +606,9 @@
     <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000145</t>
   </si>
   <si>
-    <t>NFDI4PSO:1000139</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000139</t>
-  </si>
-  <si>
-    <t>MS:1002120</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/MS_1002120</t>
-  </si>
-  <si>
     <t>MS:1001814</t>
   </si>
   <si>
@@ -719,12 +684,6 @@
     <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000119</t>
   </si>
   <si>
-    <t>NFDI4PSO:1000114</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_1000114</t>
-  </si>
-  <si>
     <t>NFDI4PSO:1000115</t>
   </si>
   <si>
@@ -812,21 +771,9 @@
     <t>n</t>
   </si>
   <si>
-    <t>STUDY DESCRIPTION_Study Type</t>
-  </si>
-  <si>
-    <t>for screen: high content screen; for experiment:  # look up in https://www.ebi.ac.uk/ols/ontologies/efo or leave blank</t>
-  </si>
-  <si>
     <t>cv</t>
   </si>
   <si>
-    <t>SCREEN/EXPERIMENT SECTION_Screen Number | Experiment Number</t>
-  </si>
-  <si>
-    <t>enter '1' for the first screen/experiment, '2' for the second etc</t>
-  </si>
-  <si>
     <t>Screen/Experiment File_Experimental conditions | Annotations_Experimental factor</t>
   </si>
   <si>
@@ -863,15 +810,9 @@
     <t>Protocol_treatment_Description</t>
   </si>
   <si>
-    <t>Screen/Experiment_Technology type</t>
-  </si>
-  <si>
     <t>cv | s</t>
   </si>
   <si>
-    <t>This is only mandatory for submissions to the collection "BioImages".</t>
-  </si>
-  <si>
     <t>Screen/Experiment_Type</t>
   </si>
   <si>
@@ -935,12 +876,6 @@
     <t>image acquistion and feature extraction protocol</t>
   </si>
   <si>
-    <t>SCREEN/EXPERIMENT SECTION_Screen Technology Type</t>
-  </si>
-  <si>
-    <t>choose from: RNAi screen, gene deletion screen, protein screen, compound screen, antibody screen, ORF overexpression screen, or enter your own value</t>
-  </si>
-  <si>
     <t>SCREEN/EXPERIMENT SECTION_Screen Type</t>
   </si>
   <si>
@@ -1058,9 +993,6 @@
     <t>shoot without leaves</t>
   </si>
   <si>
-    <t>protein localization</t>
-  </si>
-  <si>
     <t>compound treatment</t>
   </si>
   <si>
@@ -1097,9 +1029,6 @@
     <t>nailpolish</t>
   </si>
   <si>
-    <t>gene deletion screen</t>
-  </si>
-  <si>
     <t>primary screen</t>
   </si>
   <si>
@@ -1151,9 +1080,6 @@
     <t>extract archargonia from gametophyte</t>
   </si>
   <si>
-    <t>high content screen</t>
-  </si>
-  <si>
     <t>antibody target</t>
   </si>
   <si>
@@ -1163,9 +1089,6 @@
     <t>GFP:endogenous alpha tubulin 2;Cascade blue:growth media</t>
   </si>
   <si>
-    <t>compound screen</t>
-  </si>
-  <si>
     <t>secondary screen</t>
   </si>
   <si>
@@ -1208,12 +1131,6 @@
     <t>fail</t>
   </si>
   <si>
-    <t>time-lapse imaging</t>
-  </si>
-  <si>
-    <t>RNAi screen</t>
-  </si>
-  <si>
     <t>validation screen</t>
   </si>
   <si>
@@ -1232,12 +1149,6 @@
     <t>no cells</t>
   </si>
   <si>
-    <t>image cytometry</t>
-  </si>
-  <si>
-    <t>protein screen</t>
-  </si>
-  <si>
     <t>HA-Flag protein fusion library</t>
   </si>
   <si>
@@ -1248,6 +1159,9 @@
   </si>
   <si>
     <t>1.0.2</t>
+  </si>
+  <si>
+    <t>Characteristics [prepared organism part]</t>
   </si>
 </sst>
 </file>
@@ -1479,22 +1393,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A44DFED-6FA7-46AF-B778-EFE22193F0A0}" name="annotationTableFuzzyDodo24" displayName="annotationTableFuzzyDodo24" ref="A1:DL6" totalsRowShown="0">
-  <autoFilter ref="A1:DL6" xr:uid="{7A44DFED-6FA7-46AF-B778-EFE22193F0A0}"/>
-  <tableColumns count="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7A44DFED-6FA7-46AF-B778-EFE22193F0A0}" name="annotationTableFuzzyDodo24" displayName="annotationTableFuzzyDodo24" ref="A1:DC6" totalsRowShown="0">
+  <autoFilter ref="A1:DC6" xr:uid="{7A44DFED-6FA7-46AF-B778-EFE22193F0A0}"/>
+  <tableColumns count="107">
     <tableColumn id="1" xr3:uid="{DE9BEB74-08E0-478B-A4DE-942BC7303645}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{53472B8D-A3E1-44AA-9929-726B4F112D5D}" name="Parameter [microscopy sample preparation]"/>
     <tableColumn id="4" xr3:uid="{A5295512-8F1B-4B1B-B7D1-2F211EB2927E}" name="Term Source REF (NFDI4PSO:1000143)"/>
     <tableColumn id="5" xr3:uid="{3485B6B4-00D4-45BD-B9A0-B528CA1D2829}" name="Term Accession Number (NFDI4PSO:1000143)"/>
-    <tableColumn id="6" xr3:uid="{6A82CAAF-69A0-4372-86B5-B3CED79238E8}" name="Parameter [prepared organism part]"/>
+    <tableColumn id="6" xr3:uid="{6A82CAAF-69A0-4372-86B5-B3CED79238E8}" name="Characteristics [prepared organism part]"/>
     <tableColumn id="7" xr3:uid="{11A28BF1-8555-4E0C-BCD3-502CB624EFFD}" name="Term Source REF (NFDI4PSO:1000145)"/>
     <tableColumn id="8" xr3:uid="{6B4AFA59-744F-4E29-8F32-D181B223F6D3}" name="Term Accession Number (NFDI4PSO:1000145)"/>
-    <tableColumn id="9" xr3:uid="{1819CF7A-62FA-457E-BB63-969C4BE33C13}" name="Parameter [Microscopy study type]"/>
-    <tableColumn id="10" xr3:uid="{006A4740-37EE-4B48-AC52-AA7F37523433}" name="Term Source REF (NFDI4PSO:1000139)"/>
-    <tableColumn id="11" xr3:uid="{D3869B92-16AC-49E0-8841-0A6A5598E309}" name="Term Accession Number (NFDI4PSO:1000139)"/>
-    <tableColumn id="12" xr3:uid="{EAB80A3F-0921-4ECD-BA1A-57B242B5445A}" name="Parameter [experiment name]"/>
-    <tableColumn id="13" xr3:uid="{64EDBE4C-8D5B-4989-8813-33BBD4125B17}" name="Term Source REF (MS:1002120)"/>
-    <tableColumn id="14" xr3:uid="{91F864DF-1ED5-4B6D-BEDF-6A1A1A267EBB}" name="Term Accession Number (MS:1002120)"/>
     <tableColumn id="15" xr3:uid="{E60EC25B-14FC-49A1-A5D1-D34A83B91475}" name="Parameter [generic experimental condition]"/>
     <tableColumn id="16" xr3:uid="{821E867C-542E-4360-BE4A-E6FA671E60CE}" name="Term Source REF (MS:1001814)"/>
     <tableColumn id="17" xr3:uid="{E34D7500-4BCF-47D6-9258-047ED0DC2443}" name="Term Accession Number (MS:1001814)"/>
@@ -1531,9 +1439,6 @@
     <tableColumn id="48" xr3:uid="{8ABAC161-C4D1-4A59-96C8-0134D1298F19}" name="Parameter [Cover slip preparation (procedure)]"/>
     <tableColumn id="49" xr3:uid="{C0491329-5AD1-431D-AE86-50FAEFEF6D70}" name="Term Source REF (NFDI4PSO:1000119)"/>
     <tableColumn id="50" xr3:uid="{66722969-948C-41DA-9883-D5F134A5B5DD}" name="Term Accession Number (NFDI4PSO:1000119)"/>
-    <tableColumn id="51" xr3:uid="{783B102D-B4F2-4A0A-A9DB-3B84958A32FF}" name="Parameter [Screen Technology Type]"/>
-    <tableColumn id="52" xr3:uid="{61F6EAAE-CE22-4656-948D-CF8A16147609}" name="Term Source REF (NFDI4PSO:1000114)"/>
-    <tableColumn id="53" xr3:uid="{F75F2DB1-F4C5-4C63-864F-B15D81DF5FDF}" name="Term Accession Number (NFDI4PSO:1000114)"/>
     <tableColumn id="54" xr3:uid="{F473EC21-6A05-4D5A-8F9B-5527D4319ED0}" name="Parameter [high content screening stage]"/>
     <tableColumn id="55" xr3:uid="{C7163601-6E5E-43DC-B38E-D63B843DABAB}" name="Term Source REF (NFDI4PSO:1000115)"/>
     <tableColumn id="56" xr3:uid="{E4F582C5-151F-45FE-8DB5-BBD70C147C46}" name="Term Accession Number (NFDI4PSO:1000115)"/>
@@ -1908,9 +1813,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DL6"/>
+  <dimension ref="A1:DE6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="DJ1" sqref="DJ1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1918,121 +1825,112 @@
     <col min="2" max="2" width="42.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5703125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="43" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="43" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="37.5703125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="30.5703125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="37.5703125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="41" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.5703125" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="37.5703125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="41" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="34" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="41" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="29.5703125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="40" max="40" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="34" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="41" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="45.85546875" customWidth="1"/>
+    <col min="42" max="42" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="40.42578125" customWidth="1"/>
     <col min="45" max="45" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="46" max="46" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="49" max="49" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="49" max="49" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="28" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="52" max="52" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="53" max="53" width="40.42578125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="55" max="55" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="56" max="56" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="30.85546875" hidden="1" customWidth="1"/>
     <col min="58" max="58" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="28" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="59" max="59" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="19.85546875" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="26.85546875" hidden="1" customWidth="1"/>
     <col min="62" max="62" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="19.85546875" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="26.85546875" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="64" max="64" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="65" max="65" width="29" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="73" max="73" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="74" max="74" width="29" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="52.42578125" bestFit="1" customWidth="1"/>
     <col min="75" max="75" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="76" max="76" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="77" max="77" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="30" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="79" max="79" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="81" max="81" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="82" max="82" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="83" max="83" width="52.42578125" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="84" max="84" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="85" max="85" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="30" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="88" max="88" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="89" max="89" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="92" max="92" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="30.85546875" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="37.85546875" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="32.5703125" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="39.7109375" hidden="1" customWidth="1"/>
+    <col min="92" max="92" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="93" max="93" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="94" max="94" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="95" max="95" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="30.85546875" hidden="1" customWidth="1"/>
-    <col min="97" max="97" width="37.85546875" hidden="1" customWidth="1"/>
-    <col min="98" max="98" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="32.5703125" hidden="1" customWidth="1"/>
-    <col min="100" max="100" width="39.7109375" hidden="1" customWidth="1"/>
-    <col min="101" max="101" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="26" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="97" max="97" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="98" max="98" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="36.7109375" hidden="1" customWidth="1"/>
+    <col min="100" max="100" width="43.7109375" hidden="1" customWidth="1"/>
+    <col min="101" max="101" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="103" max="103" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="104" max="104" width="26" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="36.7109375" hidden="1" customWidth="1"/>
     <col min="106" max="106" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="107" max="107" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="109" max="109" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="112" max="112" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="113" max="113" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="115" max="115" width="43.7109375" hidden="1" customWidth="1"/>
-    <col min="116" max="116" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="107" max="107" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:116" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:107" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2046,569 +1944,518 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
+        <v>365</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>45</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>46</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>48</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>49</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>50</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>51</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>52</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>54</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>55</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>56</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>57</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>58</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>59</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>60</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>61</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>62</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>63</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>64</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>65</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>67</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>68</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>69</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>70</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>71</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>72</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>73</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BW1" t="s">
         <v>74</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BX1" t="s">
         <v>75</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BY1" t="s">
         <v>76</v>
       </c>
-      <c r="BY1" t="s">
+      <c r="BZ1" t="s">
         <v>77</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>78</v>
       </c>
-      <c r="CA1" t="s">
+      <c r="CB1" t="s">
         <v>79</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>80</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>81</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>82</v>
       </c>
-      <c r="CE1" t="s">
+      <c r="CF1" t="s">
         <v>83</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CG1" t="s">
         <v>84</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>85</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CI1" t="s">
         <v>86</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>87</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>88</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>89</v>
       </c>
-      <c r="CL1" t="s">
+      <c r="CM1" t="s">
         <v>90</v>
       </c>
-      <c r="CM1" t="s">
+      <c r="CN1" t="s">
         <v>91</v>
       </c>
-      <c r="CN1" t="s">
+      <c r="CO1" t="s">
         <v>92</v>
       </c>
-      <c r="CO1" t="s">
+      <c r="CP1" t="s">
         <v>93</v>
       </c>
-      <c r="CP1" t="s">
+      <c r="CQ1" t="s">
         <v>94</v>
       </c>
-      <c r="CQ1" t="s">
+      <c r="CR1" t="s">
         <v>95</v>
       </c>
-      <c r="CR1" t="s">
+      <c r="CS1" t="s">
         <v>96</v>
       </c>
-      <c r="CS1" t="s">
+      <c r="CT1" t="s">
         <v>97</v>
       </c>
-      <c r="CT1" t="s">
+      <c r="CU1" t="s">
         <v>98</v>
       </c>
-      <c r="CU1" t="s">
+      <c r="CV1" t="s">
         <v>99</v>
       </c>
-      <c r="CV1" t="s">
+      <c r="CW1" t="s">
         <v>100</v>
       </c>
-      <c r="CW1" t="s">
+      <c r="CX1" t="s">
         <v>101</v>
       </c>
-      <c r="CX1" t="s">
+      <c r="CY1" t="s">
         <v>102</v>
       </c>
-      <c r="CY1" t="s">
+      <c r="CZ1" t="s">
         <v>103</v>
       </c>
-      <c r="CZ1" t="s">
+      <c r="DA1" t="s">
         <v>104</v>
       </c>
-      <c r="DA1" t="s">
+      <c r="DB1" t="s">
         <v>105</v>
       </c>
-      <c r="DB1" t="s">
-        <v>106</v>
-      </c>
       <c r="DC1" t="s">
-        <v>107</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>108</v>
-      </c>
-      <c r="DE1" t="s">
-        <v>109</v>
-      </c>
-      <c r="DF1" t="s">
-        <v>110</v>
-      </c>
-      <c r="DG1" t="s">
-        <v>111</v>
-      </c>
-      <c r="DH1" t="s">
-        <v>112</v>
-      </c>
-      <c r="DI1" t="s">
-        <v>113</v>
-      </c>
-      <c r="DJ1" t="s">
-        <v>114</v>
-      </c>
-      <c r="DK1" t="s">
-        <v>115</v>
-      </c>
-      <c r="DL1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:116" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H2" t="s">
+        <v>309</v>
+      </c>
+      <c r="K2" t="s">
+        <v>310</v>
+      </c>
+      <c r="N2" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>312</v>
+      </c>
+      <c r="T2" t="s">
+        <v>313</v>
+      </c>
+      <c r="W2" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>315</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>316</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>317</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>318</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>319</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>320</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>321</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>322</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>323</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>324</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>325</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>326</v>
+      </c>
+      <c r="BJ2">
+        <v>1</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>327</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>328</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>329</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>315</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>330</v>
+      </c>
+      <c r="CB2">
+        <v>78875</v>
+      </c>
+      <c r="CE2" t="s">
         <v>331</v>
       </c>
-      <c r="E2" t="s">
+      <c r="CH2" t="s">
         <v>332</v>
       </c>
-      <c r="H2" t="s">
+      <c r="CK2" t="s">
         <v>333</v>
       </c>
-      <c r="N2" t="s">
+      <c r="CN2">
+        <v>9994</v>
+      </c>
+      <c r="CQ2" t="s">
         <v>334</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="CT2" t="s">
         <v>335</v>
       </c>
-      <c r="T2" t="s">
+      <c r="CW2" t="s">
         <v>336</v>
       </c>
-      <c r="W2" t="s">
+    </row>
+    <row r="3" spans="1:107" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>337</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="H3" t="s">
         <v>338</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="K3" t="s">
         <v>339</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="Q3" t="s">
         <v>340</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="T3">
+        <v>84240</v>
+      </c>
+      <c r="AR3" t="s">
         <v>341</v>
       </c>
-      <c r="AL2" t="s">
+      <c r="AU3" t="s">
         <v>342</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AX3" t="s">
         <v>343</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="BA3" t="s">
         <v>344</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="BD3">
+        <v>1921</v>
+      </c>
+      <c r="BG3" t="s">
         <v>345</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BJ3" t="s">
         <v>346</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BM3" t="s">
         <v>347</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BP3" t="s">
         <v>348</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BS3" t="s">
         <v>349</v>
       </c>
-      <c r="BJ2" t="s">
+      <c r="BY3" t="s">
         <v>350</v>
       </c>
-      <c r="BM2" t="s">
+      <c r="CB3">
+        <v>78955</v>
+      </c>
+      <c r="CE3" t="s">
         <v>351</v>
       </c>
-      <c r="BP2" t="s">
+      <c r="CN3">
+        <v>168</v>
+      </c>
+      <c r="CQ3" t="s">
         <v>352</v>
       </c>
-      <c r="BS2">
-        <v>1</v>
-      </c>
-      <c r="BV2" t="s">
+      <c r="CT3" t="s">
         <v>353</v>
       </c>
-      <c r="BY2" t="s">
+      <c r="CW3" t="s">
         <v>354</v>
       </c>
-      <c r="CB2" t="s">
+    </row>
+    <row r="4" spans="1:107" x14ac:dyDescent="0.25">
+      <c r="AR4" t="s">
         <v>355</v>
       </c>
-      <c r="CE2" t="s">
-        <v>340</v>
-      </c>
-      <c r="CH2" t="s">
+      <c r="AU4" t="s">
         <v>356</v>
       </c>
-      <c r="CK2">
-        <v>78875</v>
-      </c>
-      <c r="CN2" t="s">
+      <c r="CE4" t="s">
         <v>357</v>
       </c>
-      <c r="CQ2" t="s">
+      <c r="CQ4" t="s">
         <v>358</v>
       </c>
-      <c r="CT2" t="s">
+      <c r="CT4" t="s">
         <v>359</v>
       </c>
-      <c r="CW2">
-        <v>9994</v>
-      </c>
-      <c r="CZ2" t="s">
+      <c r="CW4" t="s">
         <v>360</v>
       </c>
-      <c r="DC2" t="s">
+    </row>
+    <row r="5" spans="1:107" x14ac:dyDescent="0.25">
+      <c r="AU5" t="s">
         <v>361</v>
       </c>
-      <c r="DF2" t="s">
+      <c r="CT5" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:116" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="6" spans="1:107" x14ac:dyDescent="0.25">
+      <c r="CT6" t="s">
         <v>363</v>
-      </c>
-      <c r="H3" t="s">
-        <v>364</v>
-      </c>
-      <c r="N3" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>366</v>
-      </c>
-      <c r="W3" t="s">
-        <v>367</v>
-      </c>
-      <c r="Z3">
-        <v>84240</v>
-      </c>
-      <c r="AX3" t="s">
-        <v>368</v>
-      </c>
-      <c r="BA3" t="s">
-        <v>369</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>370</v>
-      </c>
-      <c r="BG3" t="s">
-        <v>371</v>
-      </c>
-      <c r="BJ3" t="s">
-        <v>372</v>
-      </c>
-      <c r="BM3">
-        <v>1921</v>
-      </c>
-      <c r="BP3" t="s">
-        <v>373</v>
-      </c>
-      <c r="BS3" t="s">
-        <v>374</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>375</v>
-      </c>
-      <c r="BY3" t="s">
-        <v>376</v>
-      </c>
-      <c r="CB3" t="s">
-        <v>377</v>
-      </c>
-      <c r="CH3" t="s">
-        <v>378</v>
-      </c>
-      <c r="CK3">
-        <v>78955</v>
-      </c>
-      <c r="CN3" t="s">
-        <v>379</v>
-      </c>
-      <c r="CW3">
-        <v>168</v>
-      </c>
-      <c r="CZ3" t="s">
-        <v>380</v>
-      </c>
-      <c r="DC3" t="s">
-        <v>381</v>
-      </c>
-      <c r="DF3" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="4" spans="1:116" x14ac:dyDescent="0.25">
-      <c r="H4" t="s">
-        <v>383</v>
-      </c>
-      <c r="AX4" t="s">
-        <v>384</v>
-      </c>
-      <c r="BA4" t="s">
-        <v>385</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>386</v>
-      </c>
-      <c r="CN4" t="s">
-        <v>387</v>
-      </c>
-      <c r="CZ4" t="s">
-        <v>388</v>
-      </c>
-      <c r="DC4" t="s">
-        <v>389</v>
-      </c>
-      <c r="DF4" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="5" spans="1:116" x14ac:dyDescent="0.25">
-      <c r="H5" t="s">
-        <v>391</v>
-      </c>
-      <c r="AX5" t="s">
-        <v>392</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>393</v>
-      </c>
-      <c r="DC5" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" spans="1:116" x14ac:dyDescent="0.25">
-      <c r="DC6" t="s">
-        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -2623,7 +2470,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BFC1F7F-AF17-4F06-B9F6-D890583989BE}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2634,197 +2483,197 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>396</v>
+        <v>364</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B5" s="8"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B6" s="8"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B16" s="9"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B19" s="8"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B22" s="8"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B23" s="8"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B24" s="8"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B25" s="9"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B26" s="10"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B27" s="8"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B28" s="11"/>
     </row>
@@ -2836,9 +2685,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4249ADA-E892-40D4-A1B2-AA62559F2C3F}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2858,40 +2709,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -2915,20 +2766,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -2936,23 +2787,23 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>5</v>
+        <v>365</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -2960,1097 +2811,1007 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>252</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="H5" s="13"/>
       <c r="I5" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>253</v>
+        <v>157</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>255</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="H6" s="13"/>
       <c r="I6" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="K6" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K6" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K7" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
-        <v>257</v>
+        <v>239</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K8" s="13" t="s">
-        <v>258</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="H9" s="13"/>
+        <v>240</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>241</v>
+      </c>
       <c r="I9" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="L9" s="13"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="H10" s="13"/>
+        <v>243</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>244</v>
+      </c>
       <c r="I10" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K10" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>242</v>
+      </c>
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
       <c r="I11" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K11" s="13" t="s">
-        <v>262</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K11" s="13"/>
       <c r="L11" s="13"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>264</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="H12" s="13"/>
       <c r="I12" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="L12" s="13"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>266</v>
-      </c>
+        <v>247</v>
+      </c>
+      <c r="H13" s="13"/>
       <c r="I13" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K13" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K13" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L14" s="13"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L15" s="13"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
-        <v>267</v>
+        <v>247</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J16" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="s">
-        <v>267</v>
+        <v>249</v>
       </c>
       <c r="H17" s="13"/>
       <c r="I17" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>258</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J18" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K18" s="13" t="s">
-        <v>258</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K18" s="13"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13" t="s">
-        <v>268</v>
+        <v>251</v>
       </c>
       <c r="H19" s="13"/>
       <c r="I19" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>269</v>
+        <v>157</v>
       </c>
       <c r="K19" s="13" t="s">
-        <v>270</v>
+        <v>252</v>
       </c>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13" t="s">
-        <v>271</v>
+        <v>253</v>
       </c>
       <c r="H20" s="13"/>
       <c r="I20" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="K20" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K20" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13" t="s">
-        <v>272</v>
+        <v>255</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K21" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K21" s="13" t="s">
+        <v>238</v>
+      </c>
       <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13" t="s">
-        <v>273</v>
+        <v>256</v>
       </c>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K22" s="13" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13" t="s">
-        <v>275</v>
+        <v>257</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K23" s="13" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13" t="s">
-        <v>277</v>
+        <v>258</v>
       </c>
       <c r="H24" s="13"/>
       <c r="I24" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13" t="s">
-        <v>278</v>
+        <v>258</v>
       </c>
       <c r="H25" s="13"/>
       <c r="I25" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>244</v>
+        <v>161</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>245</v>
+        <v>169</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13" t="s">
-        <v>280</v>
+        <v>260</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J31" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>246</v>
+        <v>162</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>168</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>247</v>
+        <v>170</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13" t="s">
-        <v>281</v>
+        <v>261</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J32" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K32" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>249</v>
+        <v>171</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J33" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K33" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J34" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K34" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J35" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K35" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13" t="s">
-        <v>280</v>
+        <v>262</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K36" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13" t="s">
-        <v>280</v>
+        <v>263</v>
       </c>
       <c r="H37" s="13"/>
       <c r="I37" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K37" s="13" t="s">
-        <v>258</v>
+        <v>238</v>
       </c>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>107</v>
+      <c r="A38" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>183</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="13" t="s">
-        <v>280</v>
-      </c>
+      <c r="G38" s="13"/>
       <c r="H38" s="13"/>
-      <c r="I38" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>258</v>
-      </c>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
       <c r="L38" s="13"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="L39" s="13"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="L40" s="13"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -4059,9 +3820,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F07F4D60-B166-4D21-ACEA-A455B5E396EB}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4081,40 +3844,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="K1" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>155</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>157</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>159</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>161</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -4138,20 +3901,20 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="J3" s="13"/>
       <c r="K3" s="13"/>
@@ -4159,23 +3922,23 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>5</v>
+        <v>365</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
@@ -4183,42 +3946,52 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
+      <c r="G5" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>193</v>
+        <v>158</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>266</v>
+      </c>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
@@ -4227,76 +4000,74 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13" t="s">
-        <v>286</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>287</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>167</v>
-      </c>
+        <v>266</v>
+      </c>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13" t="s">
-        <v>288</v>
-      </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
+        <v>267</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="13" t="s">
-        <v>288</v>
-      </c>
+      <c r="G9" s="13"/>
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
@@ -4305,46 +4076,38 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="13" t="s">
-        <v>289</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>290</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>167</v>
-      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
@@ -4357,20 +4120,22 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
+      <c r="G12" s="13" t="s">
+        <v>269</v>
+      </c>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="13"/>
@@ -4379,20 +4144,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="G13" s="13" t="s">
+        <v>269</v>
+      </c>
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
       <c r="J13" s="13"/>
@@ -4401,21 +4168,21 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
@@ -4425,21 +4192,21 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
@@ -4449,21 +4216,21 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>214</v>
+        <v>158</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
@@ -4473,721 +4240,643 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
+        <v>270</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>248</v>
+      </c>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13" t="s">
-        <v>291</v>
-      </c>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+        <v>272</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>248</v>
+      </c>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="I19" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J19" s="13" t="s">
-        <v>269</v>
+        <v>157</v>
       </c>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13" t="s">
-        <v>294</v>
+        <v>276</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="I20" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J20" s="13" t="s">
-        <v>269</v>
+        <v>157</v>
       </c>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13" t="s">
-        <v>296</v>
+        <v>278</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="J21" s="13" t="s">
-        <v>269</v>
+        <v>157</v>
       </c>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="J22" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K22" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K22" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="L22" s="13"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="J23" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K23" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K23" s="13" t="s">
+        <v>282</v>
+      </c>
       <c r="L23" s="13"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13" t="s">
-        <v>302</v>
+        <v>285</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>303</v>
+        <v>286</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13" t="s">
-        <v>304</v>
+        <v>287</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>306</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K25" s="13"/>
       <c r="L25" s="13"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>306</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K26" s="13"/>
       <c r="L26" s="13"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13" t="s">
-        <v>309</v>
+        <v>291</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>310</v>
+        <v>292</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>312</v>
+        <v>286</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K28" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K28" s="13" t="s">
+        <v>294</v>
+      </c>
       <c r="L28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13" t="s">
-        <v>313</v>
+        <v>295</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>314</v>
+        <v>286</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K29" s="13"/>
+        <v>157</v>
+      </c>
+      <c r="K29" s="13" t="s">
+        <v>294</v>
+      </c>
       <c r="L29" s="13"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13" t="s">
-        <v>315</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>316</v>
-      </c>
-      <c r="I30" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>167</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>244</v>
+        <v>161</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>245</v>
+        <v>169</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13" t="s">
-        <v>317</v>
-      </c>
-      <c r="H31" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="I31" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>318</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
       <c r="L31" s="13"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>246</v>
+        <v>162</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>168</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>247</v>
+        <v>170</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13" t="s">
-        <v>319</v>
-      </c>
-      <c r="H32" s="13" t="s">
-        <v>310</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>318</v>
-      </c>
+        <v>296</v>
+      </c>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
       <c r="L32" s="13"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D33" s="13" t="s">
-        <v>249</v>
+        <v>171</v>
       </c>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
+        <v>297</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>298</v>
+      </c>
       <c r="L33" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
+        <v>299</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>235</v>
+      </c>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="D35" s="13" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13" t="s">
-        <v>320</v>
-      </c>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
+        <v>301</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>157</v>
+      </c>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J36" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>322</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K36" s="13"/>
       <c r="L36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="13" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>324</v>
+        <v>306</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="J37" s="13" t="s">
-        <v>253</v>
+        <v>157</v>
       </c>
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
-        <v>107</v>
+      <c r="A38" s="14" t="s">
+        <v>1</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>183</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
-      <c r="G38" s="13" t="s">
-        <v>325</v>
-      </c>
-      <c r="H38" s="13" t="s">
-        <v>326</v>
-      </c>
-      <c r="I38" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>167</v>
-      </c>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13" t="s">
-        <v>327</v>
-      </c>
-      <c r="H39" s="13" t="s">
-        <v>328</v>
-      </c>
-      <c r="I39" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K39" s="13"/>
-      <c r="L39" s="13"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="C40" s="13" t="s">
-        <v>168</v>
-      </c>
-      <c r="D40" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13" t="s">
-        <v>329</v>
-      </c>
-      <c r="H40" s="13" t="s">
-        <v>330</v>
-      </c>
-      <c r="I40" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="K40" s="13"/>
-      <c r="L40" s="13"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
-      <c r="L41" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>